<commit_message>
sunny test case for benchmark added
</commit_message>
<xml_diff>
--- a/benchmarkLog/benchmarkTime.xlsx
+++ b/benchmarkLog/benchmarkTime.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Access Time</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>3/25/24 18:52</t>
+  </si>
+  <si>
+    <t>3/25/24 18:53</t>
+  </si>
+  <si>
+    <t>4/3/24 20:31</t>
   </si>
 </sst>
 </file>
@@ -907,25 +913,69 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1">
-        <v>45376.78691077418</v>
+      <c r="A42" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="2">
-        <v>0.0000000000009606481</v>
+      <c r="C42" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1">
-        <v>45376.78691077418</v>
+      <c r="A43" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="2">
-        <v>0.0000000000009606481</v>
+      <c r="C43" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>45385.855223324834</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.000000000000474537</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>45385.855223324834</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.000000000000474537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished sunny and rainy unit test cases for benchmark.go
</commit_message>
<xml_diff>
--- a/benchmarkLog/benchmarkTime.xlsx
+++ b/benchmarkLog/benchmarkTime.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Access Time</t>
   </si>
@@ -146,6 +146,45 @@
   </si>
   <si>
     <t>4/3/24 20:31</t>
+  </si>
+  <si>
+    <t>4/3/24 20:43</t>
+  </si>
+  <si>
+    <t>4/3/24 20:46</t>
+  </si>
+  <si>
+    <t>4/3/24 20:47</t>
+  </si>
+  <si>
+    <t>4/3/24 20:49</t>
+  </si>
+  <si>
+    <t>4/3/24 20:54</t>
+  </si>
+  <si>
+    <t>4/3/24 20:57</t>
+  </si>
+  <si>
+    <t>4/3/24 20:58</t>
+  </si>
+  <si>
+    <t>4/3/24 21:06</t>
+  </si>
+  <si>
+    <t>4/3/24 21:07</t>
+  </si>
+  <si>
+    <t>4/3/24 21:08</t>
+  </si>
+  <si>
+    <t>4/3/24 21:09</t>
+  </si>
+  <si>
+    <t>4/3/24 21:11</t>
+  </si>
+  <si>
+    <t>4/3/24 21:12</t>
   </si>
 </sst>
 </file>
@@ -957,24 +996,948 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1">
-        <v>45385.855223324834</v>
+      <c r="A46" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" t="s">
+        <v>23</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B79" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B81" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B87" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90" t="s">
+        <v>22</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B98" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B100" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B102" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B103" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B107" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B108" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B109" t="s">
+        <v>23</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B110" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B112" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B113" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B116" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B118" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B119" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B120" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B121" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B122" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B123" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B124" t="s">
+        <v>22</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B125" t="s">
+        <v>23</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B126" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B127" t="s">
+        <v>23</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B128" t="s">
+        <v>22</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B129" t="s">
+        <v>23</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1">
+        <v>45385.883684697146</v>
+      </c>
+      <c r="B130" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" s="2">
         <v>0.000000000000474537</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1">
-        <v>45385.855223324834</v>
-      </c>
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="2">
+    <row r="131">
+      <c r="A131" s="1">
+        <v>45385.883684697146</v>
+      </c>
+      <c r="B131" t="s">
+        <v>23</v>
+      </c>
+      <c r="C131" s="2">
         <v>0.000000000000474537</v>
       </c>
     </row>

</xml_diff>